<commit_message>
Correção do funcionamento do post
</commit_message>
<xml_diff>
--- a/Projeto_ETS_OMIE_Back/teste.xlsx
+++ b/Projeto_ETS_OMIE_Back/teste.xlsx
@@ -33,6 +33,21 @@
   </si>
   <si>
     <t xml:space="preserve">Preços</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110007405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111937242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111904125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7114168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total: 2106</t>
   </si>
 </sst>
 </file>
@@ -368,6 +383,55 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>